<commit_message>
Fitness First home page typo
</commit_message>
<xml_diff>
--- a/PT Timetable.xlsx
+++ b/PT Timetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Desktop\Bangor University Work files\ICE1411\Main Assignment\Gym Website\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Desktop\Bangor University Work files\ICE1411\Main Assignment\Gym-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5302D2-9623-42C6-856E-B83201973E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8315917A-ECFA-4363-9632-A99C95008C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AD672652-36C9-41FF-AC16-3DA3BDF54678}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>